<commit_message>
Reporte de monitoreo Abril
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Medicion y Monitoreo/Concentrado_Métricas-270215.xlsx
+++ b/qualtcom/Organizacional/Medicion y Monitoreo/Concentrado_Métricas-270215.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Desviacion de esfuerzo" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="37">
   <si>
     <t>&lt;Periodo&gt;</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Estimación</t>
   </si>
   <si>
-    <t>Reporte de monitoreo</t>
-  </si>
-  <si>
     <t>Plan de métricas</t>
   </si>
   <si>
@@ -135,6 +132,15 @@
   </si>
   <si>
     <t>Febrero</t>
+  </si>
+  <si>
+    <t>Catalogo de Servicios</t>
+  </si>
+  <si>
+    <t>Medicion-Monitoreo</t>
+  </si>
+  <si>
+    <t>Configuracion</t>
   </si>
 </sst>
 </file>
@@ -212,7 +218,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,6 +252,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE5E0EC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,7 +424,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -452,12 +464,7 @@
     <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -489,7 +496,26 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -592,63 +618,7 @@
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
     <cellStyle name="Porcentaje 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="51">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="43">
     <dxf>
       <fill>
         <patternFill>
@@ -1020,9 +990,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Desviacion de esfuerzo'!$B$20:$C$23</c:f>
+              <c:f>'Desviacion de esfuerzo'!$B$20:$C$26</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Preventivo</c:v>
@@ -1044,16 +1014,25 @@
                   <c:pt idx="2">
                     <c:v>Planeación</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Medicion-Monitoreo</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Calidad</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Configuracion</c:v>
+                  </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
             </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Desviacion de esfuerzo'!$D$20:$D$23</c:f>
+              <c:f>'Desviacion de esfuerzo'!$D$20:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>140</c:v>
                 </c:pt>
@@ -1065,6 +1044,15 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>91.200000000000017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1092,9 +1080,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Desviacion de esfuerzo'!$B$20:$C$23</c:f>
+              <c:f>'Desviacion de esfuerzo'!$B$20:$C$26</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Preventivo</c:v>
@@ -1116,16 +1104,25 @@
                   <c:pt idx="2">
                     <c:v>Planeación</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Medicion-Monitoreo</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Calidad</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Configuracion</c:v>
+                  </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
             </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Desviacion de esfuerzo'!$E$20:$E$23</c:f>
+              <c:f>'Desviacion de esfuerzo'!$E$20:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1137,6 +1134,15 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1156,11 +1162,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="3766352"/>
-        <c:axId val="3766912"/>
+        <c:axId val="561836928"/>
+        <c:axId val="561840288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="3766352"/>
+        <c:axId val="561836928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1170,7 +1176,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="3766912"/>
+        <c:crossAx val="561840288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1178,7 +1184,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3766912"/>
+        <c:axId val="561840288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1189,7 +1195,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="3766352"/>
+        <c:crossAx val="561836928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1241,7 +1247,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1305,11 +1310,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="200308672"/>
-        <c:axId val="200309232"/>
+        <c:axId val="218243200"/>
+        <c:axId val="218240400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="200308672"/>
+        <c:axId val="218243200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1319,7 +1324,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200309232"/>
+        <c:crossAx val="218240400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1327,7 +1332,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200309232"/>
+        <c:axId val="218240400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1339,7 +1344,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200308672"/>
+        <c:crossAx val="218243200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1397,7 +1402,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1410,6 +1414,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Febrero</c:v>
+          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -1456,11 +1463,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="200312032"/>
-        <c:axId val="200312592"/>
+        <c:axId val="452085472"/>
+        <c:axId val="452092752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="200312032"/>
+        <c:axId val="452085472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1470,7 +1477,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200312592"/>
+        <c:crossAx val="452092752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1478,7 +1485,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200312592"/>
+        <c:axId val="452092752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1490,7 +1497,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200312032"/>
+        <c:crossAx val="452085472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1570,9 +1577,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Desviacion de esfuerzo'!$B$20:$C$23</c:f>
+              <c:f>'Desviacion de esfuerzo'!$B$20:$C$26</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Preventivo</c:v>
@@ -1594,16 +1601,25 @@
                   <c:pt idx="2">
                     <c:v>Planeación</c:v>
                   </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Medicion-Monitoreo</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Calidad</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Configuracion</c:v>
+                  </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
             </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Desviacion de esfuerzo'!$F$20:$F$23</c:f>
+              <c:f>'Desviacion de esfuerzo'!$F$20:$F$26</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1615,6 +1631,15 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.12280701754385981</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.19999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.65999999999999992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1634,11 +1659,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="3769712"/>
-        <c:axId val="3770272"/>
+        <c:axId val="561834688"/>
+        <c:axId val="561829648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="3769712"/>
+        <c:axId val="561834688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1648,7 +1673,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="3770272"/>
+        <c:crossAx val="561829648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1656,7 +1681,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3770272"/>
+        <c:axId val="561829648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1669,7 +1694,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="3769712"/>
+        <c:crossAx val="561834688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1815,7 +1840,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4000</c:v>
+                  <c:v>4685.1000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1835,11 +1860,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="149666848"/>
-        <c:axId val="149667408"/>
+        <c:axId val="451283824"/>
+        <c:axId val="451284384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="149666848"/>
+        <c:axId val="451283824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1849,7 +1874,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149667408"/>
+        <c:crossAx val="451284384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1857,7 +1882,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149667408"/>
+        <c:axId val="451284384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1868,7 +1893,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149666848"/>
+        <c:crossAx val="451283824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1969,7 +1994,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.29747283415265569</c:v>
+                  <c:v>0.17714749382215175</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1989,11 +2014,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="149670208"/>
-        <c:axId val="149670768"/>
+        <c:axId val="451283264"/>
+        <c:axId val="451282704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="149670208"/>
+        <c:axId val="451283264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2003,7 +2028,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149670768"/>
+        <c:crossAx val="451282704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2011,7 +2036,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149670768"/>
+        <c:axId val="451282704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2024,7 +2049,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149670208"/>
+        <c:crossAx val="451283264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2071,7 +2096,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2135,11 +2159,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="149673008"/>
-        <c:axId val="149673568"/>
+        <c:axId val="451279344"/>
+        <c:axId val="451272064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="149673008"/>
+        <c:axId val="451279344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2149,7 +2173,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149673568"/>
+        <c:crossAx val="451272064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2157,7 +2181,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149673568"/>
+        <c:axId val="451272064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2168,7 +2192,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149673008"/>
+        <c:crossAx val="451279344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2221,7 +2245,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2259,13 +2282,13 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2285,11 +2308,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="149777536"/>
-        <c:axId val="149778096"/>
+        <c:axId val="556022720"/>
+        <c:axId val="556021600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="149777536"/>
+        <c:axId val="556022720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2299,7 +2322,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149778096"/>
+        <c:crossAx val="556021600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2307,7 +2330,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149778096"/>
+        <c:axId val="556021600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2319,7 +2342,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149777536"/>
+        <c:crossAx val="556022720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2372,7 +2395,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2398,7 +2420,7 @@
                   <c:v>Estimación</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Reporte de monitoreo</c:v>
+                  <c:v>Catalogo de Servicios</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2416,7 +2438,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2436,11 +2458,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="149780896"/>
-        <c:axId val="149781456"/>
+        <c:axId val="556027760"/>
+        <c:axId val="556027200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="149780896"/>
+        <c:axId val="556027760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2450,7 +2472,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149781456"/>
+        <c:crossAx val="556027200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2458,7 +2480,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="149781456"/>
+        <c:axId val="556027200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2470,7 +2492,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149780896"/>
+        <c:crossAx val="556027760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2523,7 +2545,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2564,7 +2585,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2587,11 +2608,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="175223792"/>
-        <c:axId val="175224352"/>
+        <c:axId val="441466256"/>
+        <c:axId val="441465696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="175223792"/>
+        <c:axId val="441466256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2601,7 +2622,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175224352"/>
+        <c:crossAx val="441465696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2609,7 +2630,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="175224352"/>
+        <c:axId val="441465696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2621,7 +2642,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175223792"/>
+        <c:crossAx val="441466256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2674,7 +2695,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2738,11 +2758,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="175227152"/>
-        <c:axId val="175227712"/>
+        <c:axId val="441469056"/>
+        <c:axId val="441467376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="175227152"/>
+        <c:axId val="441469056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2752,7 +2772,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175227712"/>
+        <c:crossAx val="441467376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2760,7 +2780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="175227712"/>
+        <c:axId val="441467376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2772,7 +2792,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175227152"/>
+        <c:crossAx val="441469056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2805,17 +2825,17 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>328083</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>116417</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2836,22 +2856,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>198965</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>444499</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>285751</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2894,7 +2914,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2932,7 +2952,7 @@
         <xdr:cNvPr id="3" name="2 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2975,7 +2995,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3011,7 +3031,7 @@
         <xdr:cNvPr id="7" name="6 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3052,7 +3072,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3088,7 +3108,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3129,7 +3149,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3172,7 +3192,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3519,8 +3539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E26" sqref="D24:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3556,8 +3576,8 @@
     <row r="17" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:22" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
-        <v>34</v>
+      <c r="B19" s="36" t="s">
+        <v>33</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>1</v>
@@ -3565,81 +3585,126 @@
       <c r="E19" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="38" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="34">
         <v>140</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="34">
         <v>0</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="35">
         <f>(D20-E20)/D20</f>
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="34"/>
+      <c r="B21" s="38"/>
       <c r="C21" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="34">
         <v>140</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="34">
         <v>0</v>
       </c>
-      <c r="F21" s="20">
+      <c r="F21" s="35">
         <f t="shared" ref="F21:F23" si="0">(D21-E21)/D21</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="38" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="34">
         <v>45.600000000000009</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="34">
         <v>25</v>
       </c>
-      <c r="F22" s="20">
+      <c r="F22" s="35">
         <f t="shared" si="0"/>
         <v>0.45175438596491241</v>
       </c>
     </row>
     <row r="23" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="34"/>
+      <c r="B23" s="38"/>
       <c r="C23" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="34">
         <v>91.200000000000017</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="34">
         <v>80</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="35">
         <f t="shared" si="0"/>
         <v>0.12280701754385981</v>
       </c>
     </row>
-    <row r="24" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="32"/>
+      <c r="D24" s="31">
+        <v>1</v>
+      </c>
+      <c r="E24" s="31">
+        <v>1</v>
+      </c>
+      <c r="F24" s="33">
+        <f>(D24-E24)/D24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="32"/>
+      <c r="D25" s="31">
+        <v>2</v>
+      </c>
+      <c r="E25" s="31">
+        <v>2.4</v>
+      </c>
+      <c r="F25" s="33">
+        <f t="shared" ref="F25:F26" si="1">(D25-E25)/D25</f>
+        <v>-0.19999999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="32"/>
+      <c r="D26" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="37">
+        <v>0.17</v>
+      </c>
+      <c r="F26" s="33">
+        <f t="shared" si="1"/>
+        <v>0.65999999999999992</v>
+      </c>
+    </row>
     <row r="27" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="2:22" x14ac:dyDescent="0.25">
@@ -4124,7 +4189,7 @@
     <mergeCell ref="B20:B21"/>
   </mergeCells>
   <conditionalFormatting sqref="A29:XFD1048576">
-    <cfRule type="cellIs" dxfId="50" priority="63" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="42" priority="63" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison5!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4143,8 +4208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E31"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4181,7 +4246,7 @@
     <row r="18" spans="2:5" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:5" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>1</v>
@@ -4216,11 +4281,11 @@
         <v>5693.7300000000005</v>
       </c>
       <c r="D21" s="15">
-        <v>4000</v>
+        <v>4685.1000000000004</v>
       </c>
       <c r="E21" s="16">
         <f t="shared" ref="E21" si="0">(C21-D21)/C21</f>
-        <v>0.29747283415265569</v>
+        <v>0.17714749382215175</v>
       </c>
     </row>
     <row r="22" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -4235,7 +4300,7 @@
     <row r="31" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A27:XFD1048576">
-    <cfRule type="cellIs" dxfId="49" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="41" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison5!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4250,8 +4315,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="B2:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4271,94 +4336,94 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D2" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="22" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="22"/>
-      <c r="C3" s="23" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="30">
         <v>150228</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="28"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="21">
+      <c r="B4" s="18">
         <v>1</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="23">
         <v>1</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="26">
         <f>AVERAGE(D4:F4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="21">
+      <c r="B5" s="18">
         <v>2</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="29" t="e">
+      <c r="G5" s="26" t="e">
         <f>AVERAGE(D5:F5)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="21">
+      <c r="B6" s="18">
         <v>3</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="29" t="e">
+      <c r="G6" s="26" t="e">
         <f>AVERAGE(D6:F6)</f>
         <v>#DIV/0!</v>
       </c>
@@ -4368,143 +4433,143 @@
       <c r="O7" s="5"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="25" t="s">
+      <c r="D8" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="22" t="s">
         <v>8</v>
       </c>
       <c r="O8" s="5"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="33">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="30">
         <v>150227</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="30"/>
+      <c r="G9" s="27"/>
       <c r="O9" s="5"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="21">
+      <c r="B10" s="18">
         <v>1</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="27">
-        <v>1</v>
-      </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="31">
+      <c r="D10" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="28" t="e">
         <f t="shared" ref="G10:G12" si="0">AVERAGE(D10:F10)</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="21">
+      <c r="B11" s="18">
         <v>2</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="27">
-        <v>1</v>
-      </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="31">
+      <c r="D11" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="28" t="e">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="21">
+      <c r="B12" s="18">
         <v>3</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="27">
-        <v>1</v>
-      </c>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="31">
+      <c r="D12" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="28" t="e">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="25" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A3:C3 M2:XFD6 A9:A12 A15:XFD1048576 A8:B8 A4:G6 A2:G2 A7:H7 H8 A13:H14 J7:XFD14 G9:H12">
-    <cfRule type="cellIs" dxfId="48" priority="16" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="40" priority="16" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:E8">
-    <cfRule type="cellIs" dxfId="47" priority="12" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="39" priority="12" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="46" priority="11" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="38" priority="11" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="45" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="37" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="44" priority="9" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="36" priority="9" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:F12">
-    <cfRule type="cellIs" dxfId="43" priority="7" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="35" priority="7" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C12">
-    <cfRule type="cellIs" dxfId="42" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="34" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:F3">
-    <cfRule type="cellIs" dxfId="41" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="33" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:F9">
-    <cfRule type="cellIs" dxfId="40" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="32" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="39" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="31" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="38" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="30" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4523,8 +4588,8 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="B2:I39"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4542,56 +4607,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="22" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="23" t="s">
+      <c r="B3" s="20"/>
+      <c r="C3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="30">
         <v>150228</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="28"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="23">
+      <c r="B4" s="20">
         <v>1</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="24">
         <v>1</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="28">
         <f>AVERAGE(D4:F4)</f>
         <v>1</v>
       </c>
@@ -4599,22 +4664,22 @@
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="23">
+      <c r="B5" s="20">
         <v>2</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="24">
         <v>1</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="28">
         <f>AVERAGE(D5:F5)</f>
         <v>1</v>
       </c>
@@ -4622,24 +4687,24 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="23">
+      <c r="B6" s="20">
         <v>3</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="27" t="s">
+      <c r="C6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="24">
+        <v>1</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="F6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="31" t="e">
+      <c r="G6" s="28">
         <f>AVERAGE(D6:F6)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -4650,57 +4715,57 @@
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="32" t="s">
+      <c r="D8" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="G8" s="29" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="33">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="30">
         <v>150227</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="30"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="23">
+      <c r="B10" s="20">
         <v>1</v>
       </c>
-      <c r="C10" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="26" t="s">
+      <c r="C10" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="29" t="e">
+      <c r="G10" s="26" t="e">
         <f t="shared" ref="G10:G12" si="0">AVERAGE(D10:F10)</f>
         <v>#DIV/0!</v>
       </c>
@@ -4708,45 +4773,45 @@
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="23">
+      <c r="B11" s="20">
         <v>2</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="26">
-        <v>1</v>
-      </c>
-      <c r="E11" s="26" t="s">
+      <c r="C11" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="E11" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="29">
+      <c r="F11" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="26" t="e">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="9"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="23">
+      <c r="B12" s="20">
         <v>3</v>
       </c>
-      <c r="C12" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="26" t="s">
+      <c r="C12" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="29" t="e">
+      <c r="G12" s="26" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -4788,82 +4853,82 @@
     <sortCondition descending="1" ref="C29"/>
   </sortState>
   <conditionalFormatting sqref="J2:XFD10 A2:A11 H2:I3 H11:XFD11 A13:XFD14 A18:XFD1048576 A15:B17 D15:XFD17">
-    <cfRule type="cellIs" dxfId="37" priority="20" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="29" priority="20" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3 B8 B2:G2 B7:G7 G9:G12 C4:G6">
-    <cfRule type="cellIs" dxfId="36" priority="19" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="28" priority="19" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="35" priority="16" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="27" priority="16" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:E8">
-    <cfRule type="cellIs" dxfId="34" priority="17" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="26" priority="17" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="33" priority="15" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="25" priority="15" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="32" priority="10" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="24" priority="10" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D12">
-    <cfRule type="cellIs" dxfId="31" priority="14" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="23" priority="14" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="30" priority="13" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="22" priority="13" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C12">
-    <cfRule type="cellIs" dxfId="29" priority="9" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="21" priority="9" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6">
-    <cfRule type="cellIs" dxfId="28" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="20" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:B12">
-    <cfRule type="cellIs" dxfId="27" priority="7" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="19" priority="7" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:F3">
-    <cfRule type="cellIs" dxfId="26" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="18" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:F9">
-    <cfRule type="cellIs" dxfId="25" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="17" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F12">
-    <cfRule type="cellIs" dxfId="24" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="16" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="23" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="14" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4900,56 +4965,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="32" t="s">
+      <c r="D2" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="29" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="33">
+      <c r="B3" s="20"/>
+      <c r="C3" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="30">
         <v>150227</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="28"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="23">
+      <c r="B4" s="20">
         <v>1</v>
       </c>
-      <c r="C4" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="27">
+      <c r="C4" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="24">
         <v>1</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="28">
         <f>AVERAGE(D4:F4)</f>
         <v>1</v>
       </c>
@@ -4957,22 +5022,22 @@
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="23">
+      <c r="B5" s="20">
         <v>2</v>
       </c>
-      <c r="C5" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="27">
+      <c r="C5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="24">
         <v>1</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="28">
         <f>AVERAGE(D5:F5)</f>
         <v>1</v>
       </c>
@@ -4980,22 +5045,22 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="23">
+      <c r="B6" s="20">
         <v>3</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="27" t="s">
+      <c r="C6" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="31" t="e">
+      <c r="G6" s="28" t="e">
         <f>AVERAGE(D6:F6)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5041,27 +5106,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:XFD7 A2:A7 H2:I3 A8:XFD9 A13:XFD1048576 A10:B12 D10:XFD12">
-    <cfRule type="cellIs" dxfId="21" priority="16" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="13" priority="16" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3 B2:G2 B7:G7 C4:G6">
-    <cfRule type="cellIs" dxfId="20" priority="15" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="12" priority="15" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6">
-    <cfRule type="cellIs" dxfId="19" priority="7" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="7" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:F3">
-    <cfRule type="cellIs" dxfId="18" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="10" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5093,56 +5158,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="32" t="s">
+      <c r="D2" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="29" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="33">
+      <c r="B3" s="20"/>
+      <c r="C3" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="30">
         <v>150227</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="28"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="23">
+      <c r="B4" s="20">
         <v>1</v>
       </c>
-      <c r="C4" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="27">
+      <c r="C4" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="24">
         <v>0.75</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="28">
         <f>AVERAGE(D4:F4)</f>
         <v>0.75</v>
       </c>
@@ -5150,22 +5215,22 @@
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="23">
+      <c r="B5" s="20">
         <v>2</v>
       </c>
-      <c r="C5" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="27">
+      <c r="C5" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="24">
         <v>1</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="28">
         <f>AVERAGE(D5:F5)</f>
         <v>1</v>
       </c>
@@ -5173,22 +5238,22 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="23">
+      <c r="B6" s="20">
         <v>3</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="27" t="s">
+      <c r="C6" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="31" t="e">
+      <c r="G6" s="28" t="e">
         <f>AVERAGE(D6:F6)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5234,27 +5299,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:XFD7 A2:A7 H2:I3 A8:XFD9 A13:XFD1048576 A10:B12 D10:XFD12">
-    <cfRule type="cellIs" dxfId="16" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3 B2:G2 B7:G7 C4:G6">
-    <cfRule type="cellIs" dxfId="15" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6">
-    <cfRule type="cellIs" dxfId="14" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:F3">
-    <cfRule type="cellIs" dxfId="13" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5267,8 +5332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5279,98 +5344,98 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E2" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="32" t="s">
+      <c r="E2" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="29" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="33">
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="30">
         <v>150227</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="23">
+      <c r="C4" s="20">
         <v>1</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="20">
+        <v>2</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G5" s="24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="23">
-        <v>2</v>
-      </c>
-      <c r="D5" s="23" t="s">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="20">
+        <v>3</v>
+      </c>
+      <c r="D6" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="23">
-        <v>3</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="24" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3 C2:G2 D4:G6">
-    <cfRule type="cellIs" dxfId="11" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C6">
-    <cfRule type="cellIs" dxfId="10" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G3">
-    <cfRule type="cellIs" dxfId="9" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>